<commit_message>
Added Tool Box and Metal Pipe
</commit_message>
<xml_diff>
--- a/Animation & Game Project 1/Manual_Transmission/Asset Schedule.xlsx
+++ b/Animation & Game Project 1/Manual_Transmission/Asset Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UVUFALL2019\Animation &amp; Game Project 1\Manual_Transmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AFE914-04C1-4DC7-B8C3-2F4C482F751F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E04DD0-C8BF-40EB-AABD-D692A98087CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Assets</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Obi Fluid 4 - Asset Store</t>
   </si>
 </sst>
 </file>
@@ -508,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,9 +528,10 @@
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -537,24 +544,27 @@
       <c r="E1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -563,7 +573,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -572,16 +582,16 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -590,7 +600,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -599,16 +609,16 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>12</v>
       </c>
@@ -617,42 +627,42 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>3</v>
       </c>
@@ -661,7 +671,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>26</v>
       </c>
@@ -669,63 +679,66 @@
         <v>20</v>
       </c>
       <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>8</v>
       </c>

</xml_diff>